<commit_message>
Excel Writer Code 2
</commit_message>
<xml_diff>
--- a/src/test/resources/Recipe_Scrapping_Data.xlsx
+++ b/src/test/resources/Recipe_Scrapping_Data.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kavita\ReceipeHackathon\Git_project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD8837-73B7-4666-81F0-20D576F7A441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420151F3-A1AB-457F-8874-F6429844042E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LFV" sheetId="1" r:id="rId1"/>
+    <sheet name="LCHF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -100,7 +101,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -466,143 +466,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.265625"/>
+    <col min="1" max="1" width="23.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="39.4">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A05EE6-C217-4373-B0F9-AD6E83D832D9}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="35.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>20</v>
-      </c>
     </row>
     <row r="3" spans="1:1" ht="39.4">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="1:1" ht="26.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>16</v>
-      </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>18</v>
-      </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>